<commit_message>
Fixing adding constraints from z columns that look something like 'state'.{'attribute1','attribute2'} Basically, we convert the ZColumn object's values into a SQL IN type statement, and add that as a constraint (eg. state in (attribute1, attribute2))
</commit_message>
<xml_diff>
--- a/zqlparserdemo/zqlexamples.xlsx
+++ b/zqlparserdemo/zqlexamples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20415" windowHeight="10102" tabRatio="500"/>
+    <workbookView windowWidth="20415" windowHeight="10522" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60">
   <si>
     <t>Name</t>
   </si>
@@ -154,6 +154,9 @@
     <t>v2</t>
   </si>
   <si>
+    <t>(this is cross product example</t>
+  </si>
+  <si>
     <t>^ note v1,v2 (parser can't handle a space! like v1, v2)</t>
   </si>
   <si>
@@ -167,6 +170,30 @@
   </si>
   <si>
     <t>y3&lt;-{'soldprice','listingprice'}</t>
+  </si>
+  <si>
+    <t>(this is the pairwise example)</t>
+  </si>
+  <si>
+    <t>z1&lt;-'state'.'CA'</t>
+  </si>
+  <si>
+    <t>z2&lt;-'state'.'NY'</t>
+  </si>
+  <si>
+    <t>x2,y2&lt;-argmin_{x1,y1}[k=1]DEuclidean(f1,f2)</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>'state'.{'CA','NY'}</t>
+  </si>
+  <si>
+    <t>state='NY'</t>
   </si>
 </sst>
 </file>
@@ -174,10 +201,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -208,6 +235,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -215,12 +264,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -236,6 +286,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -244,88 +349,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -345,20 +372,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,19 +406,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,133 +538,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,32 +596,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -592,37 +625,69 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -643,6 +708,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -657,13 +737,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -676,164 +769,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -846,6 +930,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1225,10 +1317,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1236,8 +1328,7 @@
     <col min="2" max="2" width="18.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="33.1666666666667" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="21.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="21.6666666666667" customWidth="1"/>
+    <col min="5" max="6" width="21.6666666666667" customWidth="1"/>
     <col min="7" max="7" width="50.7583333333333" customWidth="1"/>
     <col min="8" max="8" width="5.66666666666667" customWidth="1"/>
     <col min="9" max="9" width="74.6666666666667" customWidth="1"/>
@@ -1273,7 +1364,7 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -1291,7 +1382,6 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="1"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1329,7 +1419,6 @@
       <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2"/>
       <c r="I5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1358,7 +1447,7 @@
     </row>
     <row r="8" s="3" customFormat="1"/>
     <row r="9" spans="1:5">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1410,7 +1499,7 @@
     </row>
     <row r="12" s="1" customFormat="1"/>
     <row r="13" spans="1:5">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
@@ -1481,7 +1570,7 @@
       <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="14" t="s">
         <v>35</v>
       </c>
       <c r="G17" t="s">
@@ -1516,7 +1605,7 @@
       <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="14" t="s">
         <v>35</v>
       </c>
       <c r="G20" t="s">
@@ -1554,7 +1643,7 @@
       </c>
     </row>
     <row r="25" customFormat="1" spans="1:5">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B25" t="s">
@@ -1567,7 +1656,7 @@
         <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1590,7 +1679,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" customFormat="1" spans="1:4">
+    <row r="27" customFormat="1" spans="1:5">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1602,17 +1691,20 @@
       </c>
       <c r="D27" t="s">
         <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1"/>
     <row r="29" spans="7:7">
       <c r="G29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="7:7">
       <c r="G31" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="16.5"/>
@@ -1638,7 +1730,7 @@
         <v>18</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>20</v>
@@ -1646,10 +1738,10 @@
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" ht="16.5" spans="1:4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
@@ -1657,11 +1749,136 @@
         <v>18</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="E35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" s="1" customFormat="1" ht="16.5"/>
+    <row r="37" ht="16.5" spans="1:7">
+      <c r="A37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" ht="16.5" spans="1:7">
+      <c r="A38" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" ht="16.5" spans="1:7">
+      <c r="A39" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" ht="16.5" spans="1:7">
+      <c r="A40" s="11"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" ht="16.5" spans="1:7">
+      <c r="A41" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" ht="16.5" spans="1:7">
+      <c r="A42" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" ht="16.5" spans="1:7">
+      <c r="A43" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>